<commit_message>
2019-01-23 -Fixed small bug when using LaskerSystem_VORDAQfiles Excel spreadsheet, originally had 18 columns but deleted the last column so it can work with the new system using .mat files to hold experiment records
</commit_message>
<xml_diff>
--- a/ExpRecordExamples/LaskerSystem_VORDAQfiles_template.xlsx
+++ b/ExpRecordExamples/LaskerSystem_VORDAQfiles_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\MATLAB\VNEL\ExpRecordExamples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0ED5FB-B0CB-4A59-8FE4-14141818F8E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5592"/>
+    <workbookView xWindow="390" yWindow="90" windowWidth="16260" windowHeight="5595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -63,15 +69,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>ROOTFILENAME</t>
-  </si>
-  <si>
-    <t>File EXTENSION</t>
-  </si>
-  <si>
-    <t>[i.e., the extension of a Lasker system files, or the '.XXX' in "ROOTNAME.XXXX"</t>
-  </si>
-  <si>
     <t>Date of experiment</t>
   </si>
   <si>
@@ -120,16 +117,37 @@
     <t>Direction of starting phase (i.e., leading or lagging)</t>
   </si>
   <si>
-    <t>ROOTNAME' in "ROOTNAME.XXX" lasker system numbering</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOTE: Keep the above header. </t>
+  </si>
+  <si>
+    <t>2019-01-22-RhGiGi-RALP-.0000</t>
+  </si>
+  <si>
+    <t>GiGi</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>sinusoid-light</t>
+  </si>
+  <si>
+    <t>RALP-Axis</t>
+  </si>
+  <si>
+    <t>2019-01-22-RhGiGi-RALP-.0001</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Entire file name including number at end "ROOTNAME.XXXX"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,27 +210,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,9 +226,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -238,6 +239,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -286,7 +290,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,9 +323,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,6 +375,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -529,149 +567,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="18" max="18" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="5" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="B6">
+        <v>20190122</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>20190122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="1">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,24 +773,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>